<commit_message>
Add price for all stocks
Add price for all stocks
</commit_message>
<xml_diff>
--- a/FNCE 449 term project data/BKR/BKR Earnings surprise.xlsx
+++ b/FNCE 449 term project data/BKR/BKR Earnings surprise.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hoang.nguyen1\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/namnguyenvu/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9ACD5F4F-41DF-4C14-A845-6FF282059448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06372BC-6A77-2946-BDA7-610D09ACFA49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="200">
   <si>
     <t>Ann Date</t>
   </si>
@@ -617,13 +617,16 @@
   </si>
   <si>
     <t>-0.42%</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -765,6 +768,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1115,10 +1131,13 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="33" borderId="0" xfId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="40" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="40" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1179,9 +1198,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1219,9 +1238,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1254,9 +1273,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1289,9 +1325,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1465,70 +1518,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M44"/>
+  <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="3.85546875" customWidth="1"/>
-    <col min="5" max="13" width="10.42578125" customWidth="1"/>
+    <col min="1" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="3.83203125" customWidth="1"/>
+    <col min="5" max="13" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="N1" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1547,8 +1606,9 @@
       <c r="M3">
         <v>15.41</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -1567,8 +1627,9 @@
       <c r="M4">
         <v>21.01</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1587,8 +1648,9 @@
       <c r="M5">
         <v>22.39</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1607,8 +1669,9 @@
       <c r="M6">
         <v>22.66</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1639,8 +1702,11 @@
       <c r="M7">
         <v>22.54</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N7" s="4">
+        <v>31.28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1671,8 +1737,11 @@
       <c r="M8">
         <v>17.27</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N8" s="5">
+        <v>32.06</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -1703,8 +1772,11 @@
       <c r="M9">
         <v>18.989999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N9" s="5">
+        <v>30.85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1735,8 +1807,11 @@
       <c r="M10">
         <v>22.21</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N10" s="5">
+        <v>41.02</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" t="s">
         <v>46</v>
       </c>
@@ -1767,8 +1842,11 @@
       <c r="M11">
         <v>23.59</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" s="5">
+        <v>38.03</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1799,8 +1877,11 @@
       <c r="M12">
         <v>27.23</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" s="5">
+        <v>38.79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -1831,8 +1912,11 @@
       <c r="M13">
         <v>31.75</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N13" s="5">
+        <v>45.36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" t="s">
         <v>61</v>
       </c>
@@ -1863,8 +1947,11 @@
       <c r="M14">
         <v>27.95</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N14" s="5">
+        <v>41.91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
       <c r="A15" t="s">
         <v>66</v>
       </c>
@@ -1895,8 +1982,11 @@
       <c r="M15">
         <v>43.09</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N15" s="5">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" t="s">
         <v>71</v>
       </c>
@@ -1927,8 +2017,11 @@
       <c r="M16">
         <v>49.88</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="5">
+        <v>44.33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
       <c r="A17" t="s">
         <v>76</v>
       </c>
@@ -1959,8 +2052,11 @@
       <c r="M17">
         <v>34.369999999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="5">
+        <v>31.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -1991,8 +2087,11 @@
       <c r="M18">
         <v>27.18</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="5">
+        <v>27.45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" t="s">
         <v>86</v>
       </c>
@@ -2023,8 +2122,11 @@
       <c r="M19">
         <v>23.1</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="5">
+        <v>18.420000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" t="s">
         <v>91</v>
       </c>
@@ -2055,8 +2157,11 @@
       <c r="M20">
         <v>32.74</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="5">
+        <v>17.14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
       <c r="A21" t="s">
         <v>96</v>
       </c>
@@ -2087,8 +2192,11 @@
       <c r="M21">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="5">
+        <v>16.64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -2119,8 +2227,11 @@
       <c r="M22">
         <v>1.41</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="5">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
       <c r="A23" t="s">
         <v>105</v>
       </c>
@@ -2151,8 +2262,11 @@
       <c r="M23">
         <v>1.65</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="5">
+        <v>14.51</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" t="s">
         <v>110</v>
       </c>
@@ -2183,8 +2297,11 @@
       <c r="M24">
         <v>1.08</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="5">
+        <v>9.42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" t="s">
         <v>115</v>
       </c>
@@ -2215,8 +2332,11 @@
       <c r="M25">
         <v>28.8</v>
       </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="5">
+        <v>30.87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
       <c r="A26" t="s">
         <v>120</v>
       </c>
@@ -2247,8 +2367,11 @@
       <c r="M26">
         <v>33.619999999999997</v>
       </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N26" s="5">
+        <v>21.36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" t="s">
         <v>125</v>
       </c>
@@ -2279,8 +2402,11 @@
       <c r="M27">
         <v>31.99</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N27" s="5">
+        <v>24.42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" t="s">
         <v>129</v>
       </c>
@@ -2311,8 +2437,11 @@
       <c r="M28">
         <v>34.65</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="5">
+        <v>32.909999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" t="s">
         <v>134</v>
       </c>
@@ -2343,8 +2472,11 @@
       <c r="M29">
         <v>21.72</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N29" s="5">
+        <v>32.82</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
       <c r="A30" t="s">
         <v>139</v>
       </c>
@@ -2375,8 +2507,11 @@
       <c r="M30">
         <v>66.33</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N30" s="5">
+        <v>37.450000000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14">
       <c r="A31" t="s">
         <v>144</v>
       </c>
@@ -2407,8 +2542,11 @@
       <c r="M31">
         <v>55.98</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N31" s="5">
+        <v>44.38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -2439,8 +2577,11 @@
       <c r="M32">
         <v>42.72</v>
       </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N32" s="5">
+        <v>41.45</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
       <c r="A33" t="s">
         <v>154</v>
       </c>
@@ -2471,8 +2612,11 @@
       <c r="M33">
         <v>67.319999999999993</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N33" s="5">
+        <v>48.12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14">
       <c r="A34" t="s">
         <v>159</v>
       </c>
@@ -2497,8 +2641,11 @@
       <c r="K34" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N34" s="5">
+        <v>41.53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" t="s">
         <v>164</v>
       </c>
@@ -2523,8 +2670,11 @@
       <c r="K35" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N35" s="5">
+        <v>50.01</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" t="s">
         <v>169</v>
       </c>
@@ -2549,8 +2699,11 @@
       <c r="K36" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N36" s="5">
+        <v>47.56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
       <c r="A37" t="s">
         <v>169</v>
       </c>
@@ -2566,8 +2719,11 @@
       <c r="K37" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N37" s="5">
+        <v>47.56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -2583,8 +2739,11 @@
       <c r="K38" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N38" s="5">
+        <v>41.53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14">
       <c r="A39" t="s">
         <v>164</v>
       </c>
@@ -2600,8 +2759,11 @@
       <c r="K39" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N39" s="5">
+        <v>50.01</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14">
       <c r="A40" t="s">
         <v>169</v>
       </c>
@@ -2617,8 +2779,11 @@
       <c r="K40" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N40" s="5">
+        <v>47.56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14">
       <c r="A41" t="s">
         <v>183</v>
       </c>
@@ -2637,8 +2802,11 @@
       <c r="L41">
         <v>-1.26</v>
       </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N41" s="5">
+        <v>37.47</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14">
       <c r="A42" t="s">
         <v>187</v>
       </c>
@@ -2654,8 +2822,11 @@
       <c r="K42" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N42" s="5">
+        <v>46.75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14">
       <c r="A43" t="s">
         <v>191</v>
       </c>
@@ -2671,8 +2842,11 @@
       <c r="K43" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N43" s="5">
+        <v>52.67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" t="s">
         <v>195</v>
       </c>
@@ -2687,6 +2861,9 @@
       </c>
       <c r="K44" t="s">
         <v>198</v>
+      </c>
+      <c r="N44" s="5">
+        <v>68.37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>